<commit_message>
Adds cost object to AmazonLabOrganizers
</commit_message>
<xml_diff>
--- a/AmazonLabOrganizers.xlsx
+++ b/AmazonLabOrganizers.xlsx
@@ -2947,7 +2947,7 @@
       <c r="D28" s="77" t="n"/>
       <c r="E28" s="269" t="inlineStr">
         <is>
-          <t>Sept. 17, 2019</t>
+          <t>Sept. 27, 2019</t>
         </is>
       </c>
       <c r="F28" s="231" t="n"/>
@@ -3480,7 +3480,11 @@
           <t>COST OBJECT/WBS ELEMENT</t>
         </is>
       </c>
-      <c r="D43" s="143" t="n"/>
+      <c r="D43" s="143" t="inlineStr">
+        <is>
+          <t>26-0521-0175-005</t>
+        </is>
+      </c>
       <c r="E43" s="231" t="n"/>
       <c r="F43" s="231" t="n"/>
       <c r="G43" s="231" t="n"/>
@@ -3534,7 +3538,7 @@
       </c>
       <c r="B45" s="285" t="inlineStr">
         <is>
-          <t>Sept. 10, 2019</t>
+          <t>Sept. 20, 2019</t>
         </is>
       </c>
       <c r="C45" s="231" t="n"/>

</xml_diff>